<commit_message>
all the panel working except billings.tsx still fixing
</commit_message>
<xml_diff>
--- a/app/assets/templates/Charges Template.xlsx
+++ b/app/assets/templates/Charges Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\ojt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\ojt\JDN-meter-list\app\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA5C725-4C70-452B-9749-0A421FA51638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE08DB5-5F82-4D88-9505-9AE0795D156E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="373">
   <si>
     <t>Tenant (Remove Column)</t>
   </si>
@@ -1127,6 +1127,18 @@
   </si>
   <si>
     <t>TNT0003387 ADDESSA CORPORATION</t>
+  </si>
+  <si>
+    <t>Tax Code</t>
+  </si>
+  <si>
+    <t>Whtax Code</t>
+  </si>
+  <si>
+    <t>For Penalty</t>
+  </si>
+  <si>
+    <t>Memo</t>
   </si>
 </sst>
 </file>
@@ -1966,27 +1978,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F391"/>
+  <dimension ref="A1:J391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="62.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2005,78 +2017,90 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" t="s">
+        <v>371</v>
+      </c>
+      <c r="J1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>

</xml_diff>